<commit_message>
Commentary on what I learned
</commit_message>
<xml_diff>
--- a/CH-054 Missing Values.xlsx
+++ b/CH-054 Missing Values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46ED349-5F10-4EA1-8886-77C23C22C75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD281679-3449-4C56-8C44-9584DD385850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="12">
   <si>
     <t>Question Tables</t>
   </si>
@@ -87,6 +87,18 @@
   </si>
   <si>
     <t>Actual Progress</t>
+  </si>
+  <si>
+    <t>The key thing I learned here is how to do</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a fill-down using a function. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">It also was a good use of a multidimensional </t>
+  </si>
+  <si>
+    <t>XLOOKUP</t>
   </si>
 </sst>
 </file>
@@ -1642,8 +1654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3642244C-49B2-45DE-BFD4-6421AF9E9E19}">
   <dimension ref="A1:U98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2159,6 +2171,9 @@
       <c r="D25" s="10">
         <v>0.05</v>
       </c>
+      <c r="F25" t="s">
+        <v>8</v>
+      </c>
       <c r="H25" s="11">
         <v>45260</v>
       </c>
@@ -2180,6 +2195,9 @@
       <c r="D26" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
+      <c r="F26" t="s">
+        <v>9</v>
+      </c>
       <c r="H26" s="11">
         <v>45291</v>
       </c>
@@ -2201,6 +2219,9 @@
       <c r="D27" s="10">
         <v>0.09</v>
       </c>
+      <c r="F27" t="s">
+        <v>10</v>
+      </c>
       <c r="H27" s="11">
         <v>44957</v>
       </c>
@@ -2221,6 +2242,9 @@
       </c>
       <c r="D28" s="12">
         <v>0.09</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
       </c>
       <c r="H28" s="11">
         <v>44985</v>

</xml_diff>

<commit_message>
Add a note about being related to CH-060
</commit_message>
<xml_diff>
--- a/CH-054 Missing Values.xlsx
+++ b/CH-054 Missing Values.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD281679-3449-4C56-8C44-9584DD385850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60ABA6E-4CB1-45B2-B0C8-39E783A1F9CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="13">
   <si>
     <t>Question Tables</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>XLOOKUP</t>
+  </si>
+  <si>
+    <t>See CH-060 for a related problem</t>
   </si>
 </sst>
 </file>
@@ -1654,8 +1657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3642244C-49B2-45DE-BFD4-6421AF9E9E19}">
   <dimension ref="A1:U98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1695,6 +1698,9 @@
       <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="H2" s="9" t="s">
         <v>2</v>
       </c>

</xml_diff>